<commit_message>
update project plan, design layout
</commit_message>
<xml_diff>
--- a/BAOCAO/Project_plan/Project_plan.xlsx
+++ b/BAOCAO/Project_plan/Project_plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\HDT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Desktop\HDT\MTT\BAOCAO\Project_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8145"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectPlan" sheetId="16" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>TT</t>
   </si>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -826,7 +826,9 @@
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
@@ -839,7 +841,9 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
@@ -852,7 +856,9 @@
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
@@ -865,7 +871,9 @@
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
@@ -878,7 +886,9 @@
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
@@ -891,7 +901,9 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
@@ -904,7 +916,9 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
@@ -917,7 +931,9 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>

</xml_diff>

<commit_message>
update report project_plane, business flow, fe admin supplier
</commit_message>
<xml_diff>
--- a/BAOCAO/Project_plan/Project_plan.xlsx
+++ b/BAOCAO/Project_plan/Project_plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>TT</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Lê Nguyễn Hoài Đăng</t>
+  </si>
+  <si>
+    <t>Cả nhóm</t>
   </si>
 </sst>
 </file>
@@ -680,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -800,7 +803,7 @@
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="1"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
@@ -813,7 +816,9 @@
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
@@ -946,7 +951,7 @@
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
@@ -959,7 +964,9 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
@@ -972,7 +979,9 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
@@ -985,7 +994,9 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
@@ -998,7 +1009,9 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
@@ -1011,7 +1024,9 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
     </row>
@@ -1024,7 +1039,9 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
@@ -1037,7 +1054,9 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
@@ -1050,7 +1069,9 @@
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
@@ -1063,7 +1084,7 @@
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="1"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
@@ -1115,7 +1136,7 @@
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="1"/>
+      <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30" s="8"/>
     </row>

</xml_diff>

<commit_message>
update projectplane, fe thu kho
</commit_message>
<xml_diff>
--- a/BAOCAO/Project_plan/Project_plan.xlsx
+++ b/BAOCAO/Project_plan/Project_plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
   <si>
     <t>TT</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Cả nhóm</t>
+  </si>
+  <si>
+    <t>Hoàn thành</t>
   </si>
 </sst>
 </file>
@@ -683,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -746,7 +749,9 @@
       <c r="E3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -761,7 +766,9 @@
       <c r="E4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -776,7 +783,9 @@
       <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -791,7 +800,9 @@
       <c r="E6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -819,7 +830,9 @@
       <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -834,7 +847,9 @@
       <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -849,7 +864,9 @@
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -864,7 +881,9 @@
       <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -879,7 +898,9 @@
       <c r="E12" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -894,7 +915,9 @@
       <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -909,7 +932,9 @@
       <c r="E14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -924,7 +949,9 @@
       <c r="E15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -939,7 +966,9 @@
       <c r="E16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -967,7 +996,9 @@
       <c r="E18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -982,7 +1013,9 @@
       <c r="E19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -997,7 +1030,9 @@
       <c r="E20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1012,7 +1047,9 @@
       <c r="E21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G21" s="1"/>
     </row>
     <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1027,7 +1064,9 @@
       <c r="E22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G22" s="1"/>
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1042,7 +1081,9 @@
       <c r="E23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1057,7 +1098,9 @@
       <c r="E24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G24" s="1"/>
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1072,7 +1115,9 @@
       <c r="E25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update nhap hang, filter san pham
</commit_message>
<xml_diff>
--- a/BAOCAO/Project_plan/Project_plan.xlsx
+++ b/BAOCAO/Project_plan/Project_plan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>TT</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Hoàn thành</t>
+  </si>
+  <si>
+    <t>Hoàn Thành</t>
   </si>
 </sst>
 </file>
@@ -254,7 +257,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -273,6 +276,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1098,8 +1102,8 @@
       <c r="E24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>46</v>
+      <c r="F24" s="10">
+        <v>0.8</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1115,8 +1119,8 @@
       <c r="E25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>46</v>
+      <c r="F25" s="10">
+        <v>0.3</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1142,8 +1146,12 @@
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="E27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1155,8 +1163,12 @@
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="E28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="G28" s="1"/>
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1168,8 +1180,12 @@
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="E29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0.7</v>
+      </c>
       <c r="G29" s="1"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>